<commit_message>
Final submission with Gerber X2 for face/back plates
</commit_message>
<xml_diff>
--- a/Project Outputs for Kenwood-TS50s-Digi-Interface/BOM/Bill of Materials-Kenwood-TS50s-Digi-Interface.xlsx
+++ b/Project Outputs for Kenwood-TS50s-Digi-Interface/BOM/Bill of Materials-Kenwood-TS50s-Digi-Interface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmadu\Documents\Amateur Radio\Kenwood-TS50s-Digi-Interface\Kenwood-TS50s-Digi-Interface\Project Outputs for Kenwood-TS50s-Digi-Interface\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53BBFB8E-FE09-4271-84B9-64DD0FF2DBC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C801A839-7394-403E-B5E4-A53B1A5CB62C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21690" yWindow="-12705" windowWidth="15375" windowHeight="7875" xr2:uid="{00EF9CEE-71E5-4A74-8FE6-148696E695C1}"/>
+    <workbookView xWindow="21690" yWindow="-12705" windowWidth="15375" windowHeight="7875" xr2:uid="{E741BD02-1F3F-47E3-9F66-53B2B31AD551}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Kenwood-TS50s" sheetId="1" r:id="rId1"/>
@@ -895,7 +895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AB1B5-0A56-4DFE-85CD-F0E036516D52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CE5A1C-8657-4E44-8970-A2ECA5F0860B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>